<commit_message>
update englíh vs SOILD
</commit_message>
<xml_diff>
--- a/Document/.Net/NetCoreJWT.xlsx
+++ b/Document/.Net/NetCoreJWT.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Hung\Code\JS\Common\Document\.Net\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Common\CommonJS\Document\.Net\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA9EC1D-1C0F-4B2F-A255-645FEDCA537B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JWT" sheetId="1" r:id="rId1"/>
     <sheet name="Proxy server" sheetId="10" r:id="rId2"/>
-    <sheet name="API" sheetId="2" r:id="rId3"/>
-    <sheet name="Middleware" sheetId="5" r:id="rId4"/>
-    <sheet name="Upload File" sheetId="9" r:id="rId5"/>
-    <sheet name="Authenticate" sheetId="7" r:id="rId6"/>
-    <sheet name="Change to Bytes" sheetId="8" r:id="rId7"/>
-    <sheet name="MVC" sheetId="4" r:id="rId8"/>
-    <sheet name="StatusApi" sheetId="3" r:id="rId9"/>
-    <sheet name="Server lifetime" sheetId="6" r:id="rId10"/>
+    <sheet name="SOILD" sheetId="11" r:id="rId3"/>
+    <sheet name="API" sheetId="2" r:id="rId4"/>
+    <sheet name="Middleware" sheetId="5" r:id="rId5"/>
+    <sheet name="Upload File" sheetId="9" r:id="rId6"/>
+    <sheet name="Authenticate" sheetId="7" r:id="rId7"/>
+    <sheet name="Change to Bytes" sheetId="8" r:id="rId8"/>
+    <sheet name="MVC" sheetId="4" r:id="rId9"/>
+    <sheet name="StatusApi" sheetId="3" r:id="rId10"/>
+    <sheet name="Server lifetime" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="196">
   <si>
     <t>using Microsoft.AspNetCore.Mvc;</t>
   </si>
@@ -832,12 +834,103 @@
     <t>là viết tắt của Content Delivery Network, có thể tạm dịch là mạng phân phối nội dung. Với hệ thống các máy chủ được đặt tại nhiều nơi sẽ giúp tối ưu tốc độ website cho người truy cập, cải thiện chất lượng website.
 CDN giúp các nhà phát triển nội dung, website và ứng dụng có thể đưa những sản phẩm của họ tới khách hàng ở những nơi có khoảng cách xa về địa lý một cách nhanh nhất, thông qua việc truy cập từ những máy chủ ở gần đó.</t>
   </si>
+  <si>
+    <t>Nguyên lý đầu tiên, tương ứng với chữ S trong SOLID. Nội dung nguyên lý: Một class chỉ nên giữ 1 trách nhiệm duy nhất 
+(Chỉ có thể sửa đổi class với 1 lý do duy nhất)</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>public class ReportManager()
+{
+   public void ReadDataFromDB();
+   public void ProcessData();
+   public void PrintReport();
+}</t>
+  </si>
+  <si>
+    <t>Class này giữ tới 3 trách nhiệm: Đọc dữ liệu từ DB, xử lý dữ liệu, in kết quả. Do đó, chỉ cần ta thay đổi DB, thay đổi cách xuất kết quả, … ta sẽ phải sửa đổi class này. Càng về sau class sẽ càng phình to ra. Theo đúng nguyên lý, ta phải tách class này ra làm 3 class riêng. Tuy số lượng class nhiều hơn những việc sửa chữa sẽ đơn giản hơn, class ngắn hơn nên cũng ít bug hơn.</t>
+  </si>
+  <si>
+    <t>https://toidicodedao.com/2015/03/24/solid-la-gi-ap-dung-cac-nguyen-ly-solid-de-tro-thanh-lap-trinh-vien-code-cung/</t>
+  </si>
+  <si>
+    <t>2. Open/closed principle</t>
+  </si>
+  <si>
+    <t>1. Single responsibility principle</t>
+  </si>
+  <si>
+    <t>Theo nguyên lý này, mỗi khi ta muốn thêm chức năng,.. cho chương trình, chúng ta nên viết class mới mở rộng class cũ ( bằng cách kế thừa hoặc sở hữu class cũ) không nên sửa đổi class cũ.</t>
+  </si>
+  <si>
+    <t>explain</t>
+  </si>
+  <si>
+    <t>3. Liskov Substitution Principle</t>
+  </si>
+  <si>
+    <t>Nguyên lý thứ ba, tương ứng với chữ L trong SOLID. Nội dung nguyên lý:Trong một chương trình, các object của class con có thể thay thế class cha mà không làm thay đổi tính đúng đắn của chương trình</t>
+  </si>
+  <si>
+    <t>4. Interface Segregation Principle</t>
+  </si>
+  <si>
+    <t>Nguyên lý thứ tư, tương ứng với chữ I trong SOLID. Nội dung nguyên lý: Thay vì dùng 1 interface lớn, ta nên tách thành nhiều interface nhỏ, với nhiều mục đích cụ thể</t>
+  </si>
+  <si>
+    <t>5. Dependency inversion principle</t>
+  </si>
+  <si>
+    <t>Nguyên lý này khá dễ hiểu. Hãy tưởng tượng chúng ta có 1 interface lớn, khoảng 100 methods. Việc implements sẽ khá cực khổ, ngoài ra còn có thể dư thừa vì 1 class không cần dùng hết 100 method. Khi tách interface ra thành nhiều interface nhỏ, gồm các method liên quan tới nhau, việc implement và quản lý sẽ dễ hơn.</t>
+  </si>
+  <si>
+    <t>Hơi khó hiểu? Không sao, lúc mới đọc mình cũng vậy. Hãy tưởng tượng bạn có 1 class cha tên Vịt. Các class VịtBầu, VịtXiêm có thể kế thừa class này, chương trình chạy bình thường. Tuy nhiên nếu ta viết class VịtChạyPin, cần pin mới chạy được. Khi class này kế thừa class Vịt, vì không có pin không chạy được, sẽ gây lỗi. Đó là 1 trường hợp vi phạm nguyên lý này.</t>
+  </si>
+  <si>
+    <t>Nguyên lý cuối cùng, tương ứng với chữ D trong SOLID. Nội dung nguyên lý:
+1. Các module cấp cao không nên phụ thuộc vào các modules cấp thấp. 
+   Cả 2 nên phụ thuộc vào abstraction.
+2. Interface (abstraction) không nên phụ thuộc vào chi tiết, mà ngược lại.
+( Các class giao tiếp với nhau thông qua interface, 
+không phải thông qua implementation.)</t>
+  </si>
+  <si>
+    <t>Nguyên lý này khá lắt léo, mình sẽ lấy ví dụ thực tế. Chúng ta đều biết 2 loại đèn: đèn tròn và đèn huỳnh quang. Chúng cùng có đuôi tròn, do đó ta có thể thay thế đèn tròn bằng đèn huỳnh quanh cho nhau 1 cách dễ dàng.
+Ở đây, interface chính là đuôi tròn, implementation là bóng đèn tròn và bóng đèn huỳnh quang. Ta có thể swap dễ dàng giữa 2 loại bóng vì ổ điện chỉ quan tâm tới interface (đuôi tròn), không quan tâm tới implementation.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nguyên lý thứ hai, tương ứng với chữ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> trong SOLID. Nội dung nguyên lý: Có thể thoải mái mở rộng 1 class, nhưng không được sửa đổi bên trong class đó 
+(open for extension but closed for modification).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +994,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -929,7 +1042,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -957,12 +1070,99 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1095,7 +1295,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1138,7 +1344,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1176,7 +1388,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1214,7 +1432,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1252,7 +1476,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1290,7 +1520,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1328,7 +1564,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1366,7 +1608,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1404,7 +1652,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1447,7 +1701,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1490,7 +1750,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1528,7 +1794,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1566,7 +1838,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1604,7 +1882,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1642,7 +1926,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1685,7 +1975,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1712,53 +2008,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:D13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A2:D13" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="17"/>
-    <tableColumn id="2" name="Description" dataDxfId="16"/>
-    <tableColumn id="3" name="Note" dataDxfId="15"/>
-    <tableColumn id="4" name="Link" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Note" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Link" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A2:E11"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Contents" dataDxfId="11"/>
-    <tableColumn id="2" name="Descriptions" dataDxfId="10"/>
-    <tableColumn id="3" name="example" dataDxfId="9"/>
-    <tableColumn id="4" name="note" dataDxfId="8"/>
-    <tableColumn id="5" name="Link refence" dataDxfId="7" dataCellStyle="Hyperlink"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3703CCE7-E2D4-4952-98E0-E795F1F695D3}" name="Table5" displayName="Table5" ref="A2:D9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:D9" xr:uid="{2D9B8CF4-AB43-4DB4-9887-AB8C99AF2D7E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{105BA238-BA46-4ECA-B3FB-EDEC56F4E9FB}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{31947657-AE0B-467D-85B2-CC0FA698FEBA}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{133B7409-EF80-4EB2-8060-F1926C4E219F}" name="Example" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{31073C6C-850B-483C-BDD9-C9DF644F9594}" name="explain" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A2:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A2:E11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:E11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="View" dataDxfId="4"/>
-    <tableColumn id="2" name="Folder" dataDxfId="3"/>
-    <tableColumn id="3" name="Descriptions" dataDxfId="2"/>
-    <tableColumn id="8" name="Exmple" dataDxfId="1"/>
-    <tableColumn id="4" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Contents" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Descriptions" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="example" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="note" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Link refence" dataDxfId="13" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C4" totalsRowShown="0">
-  <autoFilter ref="A2:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A2:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:E7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="View" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Folder" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Descriptions" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Exmple" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Note" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Syntax"/>
-    <tableColumn id="2" name="StatusCode"/>
-    <tableColumn id="3" name="Description"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Syntax"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="StatusCode"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2026,25 +2335,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="17" max="17" width="36.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="17" max="17" width="36.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2052,7 +2361,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2060,7 +2369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2068,7 +2377,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2076,7 +2385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2084,7 +2393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2092,7 +2401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -2100,17 +2409,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2118,17 +2427,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -2136,7 +2445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2144,7 +2453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2152,7 +2461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2160,7 +2469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2168,7 +2477,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2176,12 +2485,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -2189,7 +2498,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2197,7 +2506,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2205,12 +2514,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2218,17 +2527,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2236,7 +2545,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2244,7 +2553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2252,7 +2561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -2260,7 +2569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -2268,7 +2577,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -2276,12 +2585,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -2289,7 +2598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -2297,7 +2606,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -2305,7 +2614,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -2313,7 +2622,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2321,12 +2630,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -2334,7 +2643,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -2342,12 +2651,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -2355,7 +2664,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -2363,7 +2672,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2371,7 +2680,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -2379,12 +2688,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q49" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -2392,42 +2701,42 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q53" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q54" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q57" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q59" t="s">
         <v>28</v>
       </c>
@@ -2439,34 +2748,90 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.21875" customWidth="1"/>
+    <col min="3" max="3" width="70.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>404</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7265625" customWidth="1"/>
+    <col min="1" max="1" width="39.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -2476,9 +2841,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.learnentityframeworkcore.com/configuration/data-annotation-attributes"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.learnentityframeworkcore.com/configuration/fluent-api"/>
-    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.learnentityframeworkcore.com/configuration/data-annotation-attributes" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.learnentityframeworkcore.com/configuration/fluent-api" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2486,28 +2851,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="21.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>164</v>
       </c>
@@ -2521,7 +2886,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>166</v>
       </c>
@@ -2532,7 +2897,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>169</v>
       </c>
@@ -2543,7 +2908,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>172</v>
       </c>
@@ -2551,7 +2916,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>175</v>
       </c>
@@ -2561,7 +2926,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -2572,24 +2937,284 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709575E4-91B9-4F01-9C16-794215A07B29}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="60.77734375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="110.44140625" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="122.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="123" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="102" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="204" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{BAEF3A42-D871-43A3-825C-155DD067FCC6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="123.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="44.26953125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="43.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="123.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.21875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>79</v>
       </c>
@@ -2606,7 +3231,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="129.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="126" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>86</v>
       </c>
@@ -2621,7 +3246,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="277.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="270" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>87</v>
       </c>
@@ -2636,7 +3261,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="351.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="342" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>90</v>
       </c>
@@ -2651,7 +3276,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -2666,7 +3291,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>103</v>
       </c>
@@ -2679,7 +3304,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>106</v>
       </c>
@@ -2692,7 +3317,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>109</v>
       </c>
@@ -2705,7 +3330,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="148" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>112</v>
       </c>
@@ -2722,7 +3347,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>114</v>
       </c>
@@ -2733,7 +3358,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" location="update"/>
+    <hyperlink ref="E3" r:id="rId1" location="update" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2743,100 +3368,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>161</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2846,43 +3450,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>160</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2892,39 +3471,85 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A2:A54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="51.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="39.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="55.26953125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="28.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="55.21875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.21875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
@@ -2941,7 +3566,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>126</v>
       </c>
@@ -2958,7 +3583,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>132</v>
       </c>
@@ -2972,7 +3597,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>146</v>
       </c>
@@ -2983,7 +3608,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
@@ -2994,7 +3619,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>148</v>
       </c>
@@ -3015,60 +3640,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C4"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
-    <col min="2" max="2" width="55.26953125" customWidth="1"/>
-    <col min="3" max="3" width="70.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>404</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update throttle and debound javascript
</commit_message>
<xml_diff>
--- a/Document/.Net/NetCoreJWT.xlsx
+++ b/Document/.Net/NetCoreJWT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="16900" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="16900" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="JWT" sheetId="1" r:id="rId1"/>
@@ -1351,10 +1351,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2059,6 +2059,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30655</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>74448</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>198188</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>12748</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30655" y="9454931"/>
+          <a:ext cx="7472223" cy="4168714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>321236</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>67250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>108100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7672295" y="9592250"/>
+          <a:ext cx="6073587" cy="4336438"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2479,13 +2555,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:D10" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:D10" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A5:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" name="Descriptions" dataDxfId="3"/>
-    <tableColumn id="3" name="Example" dataDxfId="2"/>
-    <tableColumn id="4" name="Link" dataDxfId="1"/>
+    <tableColumn id="1" name="Name" dataDxfId="3"/>
+    <tableColumn id="2" name="Descriptions" dataDxfId="2"/>
+    <tableColumn id="3" name="Example" dataDxfId="1"/>
+    <tableColumn id="4" name="Link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3225,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3478,7 +3554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3491,7 +3567,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3687,11 +3763,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
@@ -3933,7 +4009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4105,8 +4181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4207,7 +4283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update file excel: image for Filter Action
</commit_message>
<xml_diff>
--- a/Document/.Net/NetCoreJWT.xlsx
+++ b/Document/.Net/NetCoreJWT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="16900" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="16900" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="JWT" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="236">
   <si>
     <t>using Microsoft.AspNetCore.Mvc;</t>
   </si>
@@ -1173,6 +1173,12 @@
   </si>
   <si>
     <t>https://docs.microsoft.com/en-us/aspnet/core/fundamentals/localization?view=aspnetcore-5.0</t>
+  </si>
+  <si>
+    <t>Thứ tự thực hiện Filter</t>
+  </si>
+  <si>
+    <t>Thứ tự chạy filter</t>
   </si>
 </sst>
 </file>
@@ -2135,6 +2141,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>515102</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>16520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14179550"/>
+          <a:ext cx="5391902" cy="4620270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>562819</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>130682</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="19151600"/>
+          <a:ext cx="6049219" cy="3629532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4009,7 +4091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4179,10 +4261,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA54" sqref="AA54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4250,6 +4332,16 @@
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update file excel Facebook, Account CI
</commit_message>
<xml_diff>
--- a/Document/.Net/NetCoreJWT.xlsx
+++ b/Document/.Net/NetCoreJWT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="-2240" windowWidth="23040" windowHeight="12200" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="30720" yWindow="-2240" windowWidth="23040" windowHeight="12200" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="JWT" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="OWASP Cheat Sheet Series" sheetId="6" r:id="rId11"/>
     <sheet name="DJ" sheetId="12" r:id="rId12"/>
     <sheet name="Multiple Languages" sheetId="13" r:id="rId13"/>
+    <sheet name="Docker" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="239">
   <si>
     <t>using Microsoft.AspNetCore.Mvc;</t>
   </si>
@@ -1180,12 +1181,37 @@
   <si>
     <t>Thứ tự chạy filter</t>
   </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FROM mcr.microsoft.com/dotnet/core/aspnet:3.1-buster-slim AS base
+WORKDIR /app
+EXPOSE 80
+EXPOSE 443
+FROM mcr.microsoft.com/dotnet/core/sdk:3.1-buster AS build
+WORKDIR /src
+COPY ["Toastr.csproj", "."]
+RUN dotnet restore "Toastr.csproj"
+COPY . .
+RUN dotnet build "Toastr.csproj" -c Release -o /app/build
+FROM build AS publish
+RUN dotnet publish "Toastr.csproj" -c Release -o /app/publish
+FROM base AS final
+WORKDIR /app
+COPY --from=publish /app/publish .
+ENTRYPOINT ["dotnet", "Toastr.dll"]
+</t>
+  </si>
+  <si>
+    <t>Deployment with net core</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1296,6 +1322,12 @@
       <color theme="1"/>
       <name val="Ara"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1324,7 +1356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1361,12 +1393,123 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2612,54 +2755,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:D13" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:D13" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A2:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="41"/>
-    <tableColumn id="2" name="Description" dataDxfId="40"/>
-    <tableColumn id="3" name="Note" dataDxfId="39"/>
-    <tableColumn id="4" name="Link" dataDxfId="38"/>
+    <tableColumn id="1" name="Name" dataDxfId="47"/>
+    <tableColumn id="2" name="Description" dataDxfId="46"/>
+    <tableColumn id="3" name="Note" dataDxfId="45"/>
+    <tableColumn id="4" name="Link" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:D9" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:D9" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A2:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="35"/>
-    <tableColumn id="2" name="Description" dataDxfId="34"/>
-    <tableColumn id="3" name="Example" dataDxfId="33"/>
-    <tableColumn id="4" name="explain" dataDxfId="32"/>
+    <tableColumn id="1" name="Name" dataDxfId="41"/>
+    <tableColumn id="2" name="Description" dataDxfId="40"/>
+    <tableColumn id="3" name="Example" dataDxfId="39"/>
+    <tableColumn id="4" name="explain" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E11" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E11" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A2:E11"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Contents" dataDxfId="29"/>
-    <tableColumn id="2" name="Descriptions" dataDxfId="28"/>
-    <tableColumn id="3" name="example" dataDxfId="27"/>
-    <tableColumn id="4" name="note" dataDxfId="26"/>
-    <tableColumn id="5" name="Link refence" dataDxfId="25" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Contents" dataDxfId="35"/>
+    <tableColumn id="2" name="Descriptions" dataDxfId="34"/>
+    <tableColumn id="3" name="example" dataDxfId="33"/>
+    <tableColumn id="4" name="note" dataDxfId="32"/>
+    <tableColumn id="5" name="Link refence" dataDxfId="31" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E7" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E7" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A2:E7"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="View" dataDxfId="22"/>
-    <tableColumn id="2" name="Folder" dataDxfId="21"/>
-    <tableColumn id="3" name="Descriptions" dataDxfId="20"/>
-    <tableColumn id="8" name="Exmple" dataDxfId="19"/>
-    <tableColumn id="4" name="Note" dataDxfId="18"/>
+    <tableColumn id="1" name="View" dataDxfId="28"/>
+    <tableColumn id="2" name="Folder" dataDxfId="27"/>
+    <tableColumn id="3" name="Descriptions" dataDxfId="26"/>
+    <tableColumn id="8" name="Exmple" dataDxfId="25"/>
+    <tableColumn id="4" name="Note" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2678,40 +2821,53 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:E16" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:E16" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A3:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="15"/>
-    <tableColumn id="2" name="Description" dataDxfId="14"/>
-    <tableColumn id="3" name="Example" dataDxfId="13"/>
-    <tableColumn id="4" name="Prevent" dataDxfId="12"/>
-    <tableColumn id="5" name="Link" dataDxfId="11" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Name" dataDxfId="21"/>
+    <tableColumn id="2" name="Description" dataDxfId="20"/>
+    <tableColumn id="3" name="Example" dataDxfId="19"/>
+    <tableColumn id="4" name="Prevent" dataDxfId="18"/>
+    <tableColumn id="5" name="Link" dataDxfId="17" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:D14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:D14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A3:D14"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" name="Description" dataDxfId="7"/>
-    <tableColumn id="3" name="Example" dataDxfId="6"/>
-    <tableColumn id="4" name="Link" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Name" dataDxfId="14"/>
+    <tableColumn id="2" name="Description" dataDxfId="13"/>
+    <tableColumn id="3" name="Example" dataDxfId="12"/>
+    <tableColumn id="4" name="Link" dataDxfId="11" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:D10" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:D10" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A5:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="3"/>
-    <tableColumn id="2" name="Descriptions" dataDxfId="2"/>
-    <tableColumn id="3" name="Example" dataDxfId="1"/>
-    <tableColumn id="4" name="Link" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" name="Descriptions" dataDxfId="8"/>
+    <tableColumn id="3" name="Example" dataDxfId="7"/>
+    <tableColumn id="4" name="Link" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:D4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A3:D4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" name="Code" dataDxfId="3"/>
+    <tableColumn id="4" name="Note" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3451,7 +3607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3805,6 +3961,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.5"/>
+  <cols>
+    <col min="1" max="1" width="29.54296875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="89.26953125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="61.453125" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" ht="36">
+      <c r="A3" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="350">
+      <c r="A4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>